<commit_message>
Minor edits to specs
</commit_message>
<xml_diff>
--- a/docs/specifications/cas_errors.xlsx
+++ b/docs/specifications/cas_errors.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A85E301-C6E7-4CD4-83BC-E501334037A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E76EA9C-61E4-4221-B8A9-77B7DD444B5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="540" windowWidth="19065" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>Data_type</t>
   </si>
@@ -206,16 +200,82 @@
     <t>Tree species are not recorded in a clearcut</t>
   </si>
   <si>
-    <t>There are only 2 tree species and others are recorded as ""</t>
-  </si>
-  <si>
-    <t>There are only 2 tree species and others are recorded as 0</t>
-  </si>
-  <si>
-    <t>TYPE_ERROR</t>
-  </si>
-  <si>
     <t>PRECISION_ERROR</t>
+  </si>
+  <si>
+    <t>Tree species does not occur and is recorded as empty string</t>
+  </si>
+  <si>
+    <t>Tree species does not occur and is recorded as 0</t>
+  </si>
+  <si>
+    <t>Is attribute a string?</t>
+  </si>
+  <si>
+    <t>Is precision of value greater than n?</t>
+  </si>
+  <si>
+    <t>Is value within expected range of values?</t>
+  </si>
+  <si>
+    <t>Is value within expected set of values?</t>
+  </si>
+  <si>
+    <t>INVALID_TYPE</t>
+  </si>
+  <si>
+    <t>OUT_OF_RANGE</t>
+  </si>
+  <si>
+    <t>NOT_IN_SET</t>
+  </si>
+  <si>
+    <t>PRECISION_TOO_HIGH</t>
+  </si>
+  <si>
+    <t>INFINITY</t>
+  </si>
+  <si>
+    <t>SPECIES_ERROR</t>
+  </si>
+  <si>
+    <t>INVALID_STRING</t>
+  </si>
+  <si>
+    <t>INVALID_NUMBER</t>
+  </si>
+  <si>
+    <t>MISSING_STRING</t>
+  </si>
+  <si>
+    <t>MISSING_NUMBER</t>
+  </si>
+  <si>
+    <t>UNDEF_STRING</t>
+  </si>
+  <si>
+    <t>UNDEF_NUMBER</t>
+  </si>
+  <si>
+    <t>CAS04_error</t>
+  </si>
+  <si>
+    <t>CAS05_error</t>
+  </si>
+  <si>
+    <t>TT_Between</t>
+  </si>
+  <si>
+    <t>TT_GreaterThan</t>
+  </si>
+  <si>
+    <t>TT_IsString?</t>
+  </si>
+  <si>
+    <t>TT_InSet?</t>
+  </si>
+  <si>
+    <t>"Undefined"</t>
   </si>
 </sst>
 </file>
@@ -272,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -285,6 +345,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,25 +632,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -601,16 +668,19 @@
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -632,11 +702,14 @@
       <c r="G2" s="5">
         <v>-1</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -658,11 +731,14 @@
       <c r="G3" s="5">
         <v>-8888</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="5">
         <v>-8888</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -681,25 +757,28 @@
       <c r="G4" s="5">
         <v>-8888</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -707,19 +786,22 @@
       <c r="G5" s="5">
         <v>-1111</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="5">
+        <v>-1111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>60</v>
@@ -730,11 +812,14 @@
       <c r="G6" s="5">
         <v>-1111</v>
       </c>
-      <c r="H6" s="5">
-        <v>-1111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -756,11 +841,14 @@
       <c r="G7" s="5">
         <v>-9999</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="5">
         <v>-9999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
@@ -779,11 +867,14 @@
       <c r="G8" s="5">
         <v>-9999</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
@@ -796,11 +887,14 @@
       <c r="E9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="5">
+        <v>-7777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
@@ -813,11 +907,14 @@
       <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="5">
+        <v>-6666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
@@ -836,8 +933,84 @@
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -854,16 +1027,16 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -880,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -897,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -914,7 +1087,7 @@
         <v>-9999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -931,7 +1104,7 @@
         <v>-8888</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -948,7 +1121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -965,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -982,7 +1155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added error code section to cas_document.md
</commit_message>
<xml_diff>
--- a/docs/specifications/cas_errors.xlsx
+++ b/docs/specifications/cas_errors.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E88B8-04FF-4EC5-8D7F-CC615B3564B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB243FB8-CD7C-4EC7-A8A2-53B49F5DAE6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="version 3" sheetId="3" r:id="rId1"/>
-    <sheet name="version 2" sheetId="2" r:id="rId2"/>
-    <sheet name="version 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="version 2" sheetId="2" r:id="rId3"/>
+    <sheet name="version 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="137">
   <si>
     <t>CAS04_code</t>
   </si>
@@ -470,6 +471,27 @@
   </si>
   <si>
     <t>CAS_ID</t>
+  </si>
+  <si>
+    <t>Generic Small Four Char Code</t>
+  </si>
+  <si>
+    <t>Generic Large Four Char Code</t>
+  </si>
+  <si>
+    <t>Generic Small Int Code</t>
+  </si>
+  <si>
+    <t>Generic Double Code</t>
+  </si>
+  <si>
+    <t>Generic Text Code</t>
+  </si>
+  <si>
+    <t>Generic Large Int Code</t>
+  </si>
+  <si>
+    <t>Error type</t>
   </si>
 </sst>
 </file>
@@ -527,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -535,11 +557,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,6 +594,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C433B836-2E24-4019-9D1B-300F5E0548AB}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1626,6 +1695,355 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA55EC8-7307-4427-942B-5F374DD8C01A}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="10" customWidth="1"/>
+    <col min="5" max="9" width="13" style="11" customWidth="1"/>
+    <col min="10" max="10" width="15.90625" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-2222</v>
+      </c>
+      <c r="E3" s="14">
+        <v>-222222222</v>
+      </c>
+      <c r="F3" s="14">
+        <v>-32768</v>
+      </c>
+      <c r="G3" s="14">
+        <v>-2147483648</v>
+      </c>
+      <c r="H3" s="14">
+        <v>-2147483648</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-2221</v>
+      </c>
+      <c r="E4" s="14">
+        <v>-222222221</v>
+      </c>
+      <c r="F4" s="14">
+        <v>32767</v>
+      </c>
+      <c r="G4" s="14">
+        <v>2147483647</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2147483647</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-8888</v>
+      </c>
+      <c r="E6" s="14">
+        <v>-888888888</v>
+      </c>
+      <c r="F6" s="14">
+        <v>-32767</v>
+      </c>
+      <c r="G6" s="14">
+        <v>-2147483647</v>
+      </c>
+      <c r="H6" s="14">
+        <v>-2147483647</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="14">
+        <v>-8887</v>
+      </c>
+      <c r="E8" s="14">
+        <v>-888888887</v>
+      </c>
+      <c r="F8" s="14">
+        <v>-32765</v>
+      </c>
+      <c r="G8" s="14">
+        <v>-2147483645</v>
+      </c>
+      <c r="H8" s="14">
+        <v>-2147483645</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="14">
+        <v>-9999</v>
+      </c>
+      <c r="E10" s="14">
+        <v>-999999999</v>
+      </c>
+      <c r="F10" s="14">
+        <v>-32764</v>
+      </c>
+      <c r="G10" s="14">
+        <v>-2147483644</v>
+      </c>
+      <c r="H10" s="14">
+        <v>-2147483644</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="14">
+        <v>-9998</v>
+      </c>
+      <c r="E11" s="14">
+        <v>-999999998</v>
+      </c>
+      <c r="F11" s="14">
+        <v>-32763</v>
+      </c>
+      <c r="G11" s="14">
+        <v>-2147483643</v>
+      </c>
+      <c r="H11" s="14">
+        <v>-2147483643</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="14">
+        <v>-9997</v>
+      </c>
+      <c r="E12" s="14">
+        <v>-999999997</v>
+      </c>
+      <c r="F12" s="14">
+        <v>-32762</v>
+      </c>
+      <c r="G12" s="14">
+        <v>-2147483642</v>
+      </c>
+      <c r="H12" s="14">
+        <v>-2147483642</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="14">
+        <v>-9996</v>
+      </c>
+      <c r="E13" s="14">
+        <v>-999999996</v>
+      </c>
+      <c r="F13" s="14">
+        <v>-32761</v>
+      </c>
+      <c r="G13" s="14">
+        <v>-2147483641</v>
+      </c>
+      <c r="H13" s="14">
+        <v>-2147483641</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="21">
+        <v>-9995</v>
+      </c>
+      <c r="E14" s="21">
+        <v>-999999995</v>
+      </c>
+      <c r="F14" s="21">
+        <v>-32760</v>
+      </c>
+      <c r="G14" s="21">
+        <v>-2147483640</v>
+      </c>
+      <c r="H14" s="21">
+        <v>-2147483640</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555A1D9B-A9E2-433A-9109-8482AB6619C1}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -1990,7 +2408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated specific error codes
</commit_message>
<xml_diff>
--- a/docs/specifications/cas_errors.xlsx
+++ b/docs/specifications/cas_errors.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2297628B-09C6-45D1-8D88-0ACB9DA0B6D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA2333F-34F0-4B7A-BF73-F2B6F3256ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Short v3" sheetId="4" r:id="rId1"/>
     <sheet name="Long v3" sheetId="3" r:id="rId2"/>
-    <sheet name="version 2" sheetId="2" r:id="rId3"/>
-    <sheet name="version 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Specific codes" sheetId="5" r:id="rId3"/>
+    <sheet name="version 2" sheetId="2" r:id="rId4"/>
+    <sheet name="version 1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="140">
   <si>
     <t>CAS04_code</t>
   </si>
@@ -483,6 +484,24 @@
   </si>
   <si>
     <t>Double code</t>
+  </si>
+  <si>
+    <t>Not in set</t>
+  </si>
+  <si>
+    <t>Neg infinity</t>
+  </si>
+  <si>
+    <t>Pos infinity</t>
+  </si>
+  <si>
+    <t>SPECIES_1-10</t>
+  </si>
+  <si>
+    <t>SPECIES_PER_1-10</t>
+  </si>
+  <si>
+    <t>Error_type</t>
   </si>
 </sst>
 </file>
@@ -561,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -621,6 +640,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA55EC8-7307-4427-942B-5F374DD8C01A}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1274,7 +1308,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C3" sqref="C3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1971,6 +2005,323 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C733A05B-0C07-42CA-BAFC-8B5F4B6FFF4B}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-2222</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-2222</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-2221</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-2221</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-8888</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-8888</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-8888</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-8888</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-8888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-8886</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-8886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-9998</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-9998</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-9997</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-9997</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-9997</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-9997</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="2">
+        <v>-9997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-9996</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-9996</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-9996</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-9996</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-9996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555A1D9B-A9E2-433A-9109-8482AB6619C1}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2335,7 +2686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>

</xml_diff>